<commit_message>
Published state of ETDataset on September 06 2018
</commit_message>
<xml_diff>
--- a/nodes_source_analyses/energy/energy_hydrogen_steam_methane_reformer.xlsx
+++ b/nodes_source_analyses/energy/energy_hydrogen_steam_methane_reformer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marliekeverweij/Projects/etdataset/nodes_source_analyses/energy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F2483C2-F8F9-6246-A1A0-B7C6092400C8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E220464-61B3-2A4B-8AD2-F2465787E999}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="26800" tabRatio="762" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="176">
   <si>
     <t>Source</t>
   </si>
@@ -649,9 +649,6 @@
   </si>
   <si>
     <t xml:space="preserve">MW </t>
-  </si>
-  <si>
-    <t>In table 15 an efficiency of 77% is used for the SMR plant (without CCS), so looking at table 9 the capacity should be around 225 MW</t>
   </si>
   <si>
     <t>NOT USED</t>
@@ -5388,7 +5385,7 @@
   <dimension ref="A1:Q263"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
@@ -5919,7 +5916,7 @@
         <v>20</v>
       </c>
       <c r="G33" s="64" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K33" s="71"/>
       <c r="L33" s="71"/>
@@ -6010,13 +6007,11 @@
       <c r="B41" s="70"/>
       <c r="C41" s="71"/>
       <c r="E41" s="64">
+        <f>(150+300)/2</f>
         <v>225</v>
       </c>
       <c r="F41" s="64" t="s">
         <v>173</v>
-      </c>
-      <c r="G41" s="64" t="s">
-        <v>174</v>
       </c>
       <c r="K41" s="71"/>
       <c r="L41" s="71"/>
@@ -6564,7 +6559,7 @@
     <row r="112" spans="2:17">
       <c r="B112" s="70"/>
       <c r="C112" s="68" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="113" spans="2:7">
@@ -6760,7 +6755,7 @@
     <row r="157" spans="2:7">
       <c r="B157" s="70"/>
       <c r="C157" s="68" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="158" spans="2:7">
@@ -6954,7 +6949,7 @@
       <c r="A190" s="161"/>
       <c r="B190" s="177"/>
       <c r="C190" s="68" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="191" spans="1:7">

</xml_diff>